<commit_message>
new functionality: can now edit schools from markers
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14115" windowHeight="4695"/>
+    <workbookView xWindow="390" yWindow="600" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,88 +19,88 @@
     <t>Université Bordeaux 1-IUT Agen</t>
   </si>
   <si>
+    <t>IUT</t>
+  </si>
+  <si>
     <t>Agen</t>
   </si>
   <si>
+    <t>44.802614</t>
+  </si>
+  <si>
+    <t>-0.588054</t>
+  </si>
+  <si>
     <t>Université Picardie Jules Verne-IUT Aisne</t>
   </si>
   <si>
     <t>Laon</t>
   </si>
   <si>
+    <t>49.4314025</t>
+  </si>
+  <si>
+    <t>2.0899064</t>
+  </si>
+  <si>
     <t>École nationale supérieure des mines d'Albi</t>
   </si>
   <si>
+    <t>EI</t>
+  </si>
+  <si>
     <t>Albi</t>
   </si>
   <si>
+    <t>43.9207561</t>
+  </si>
+  <si>
+    <t>2.1723533</t>
+  </si>
+  <si>
     <t>Université Paul Sabatier Toulouse 3 (UPS)-IUT Paul Sabatier-Site Albi</t>
   </si>
   <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>43.5609901</t>
+  </si>
+  <si>
+    <t>1.4630574</t>
+  </si>
+  <si>
     <t>École nationale supérieure des mines d'Alès</t>
   </si>
   <si>
     <t>Alès</t>
   </si>
   <si>
+    <t>3037,1709,3754,6908</t>
+  </si>
+  <si>
+    <t>44.13225</t>
+  </si>
+  <si>
+    <t>4.089435</t>
+  </si>
+  <si>
     <t>Université de Picardie Jules Verne</t>
   </si>
   <si>
+    <t>U</t>
+  </si>
+  <si>
     <t>Amiens</t>
   </si>
   <si>
     <t>convention générale</t>
   </si>
   <si>
-    <t>44.802614</t>
-  </si>
-  <si>
-    <t>-0.588054</t>
-  </si>
-  <si>
-    <t>49.4314025</t>
-  </si>
-  <si>
-    <t>2.0899064</t>
-  </si>
-  <si>
-    <t>43.9207561</t>
-  </si>
-  <si>
-    <t>2.1723533</t>
-  </si>
-  <si>
-    <t>43.5609901</t>
-  </si>
-  <si>
-    <t>1.4630574</t>
-  </si>
-  <si>
-    <t>44.13225</t>
-  </si>
-  <si>
-    <t>4.089435</t>
-  </si>
-  <si>
     <t>49.8764069</t>
   </si>
   <si>
     <t>2.2637991</t>
-  </si>
-  <si>
-    <t>3037,1709,3754,6908</t>
-  </si>
-  <si>
-    <t>IUT</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>EC</t>
-  </si>
-  <si>
-    <t>EI</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -494,128 +494,128 @@
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="51.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" ht="51.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3">
         <v>7764</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:6" ht="51.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3">
         <v>7764</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51.75" customHeight="1" thickBot="1">
+    <row r="3" spans="1:6" ht="51.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3">
         <v>1709.3753999999999</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="51.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:6" ht="51.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <v>7764</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="51.75" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="1:6" ht="51.75" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added primary key in data.xlsx and prefill edit form
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -136,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -145,26 +145,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF808080"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF808080"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF808080"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF808080"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -174,19 +165,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,136 +472,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="51.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3">
+      <c r="E1" s="4">
         <v>7764</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="4">
         <v>7764</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="4">
         <v>1709.3753999999999</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="51.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="4">
         <v>7764</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="51.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="51.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data.xlsx is now modified when Ecole edit
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -1,39 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="390" yWindow="600" windowWidth="19815" windowHeight="7365"/>
-  </bookViews>
-  <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="125725"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="data" sheetId="1" r:id="rId1"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Université Bordeaux 1-IUT Agen</t>
   </si>
   <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Agen</t>
+  </si>
+  <si>
+    <t>7764</t>
+  </si>
+  <si>
+    <t>44.802614</t>
+  </si>
+  <si>
+    <t>-0.5880540000000565</t>
+  </si>
+  <si>
+    <t>Université Picardie Jules Verne-IUT Aisne</t>
+  </si>
+  <si>
     <t>IUT</t>
   </si>
   <si>
-    <t>Agen</t>
-  </si>
-  <si>
-    <t>44.802614</t>
-  </si>
-  <si>
-    <t>-0.588054</t>
-  </si>
-  <si>
-    <t>Université Picardie Jules Verne-IUT Aisne</t>
-  </si>
-  <si>
     <t>Laon</t>
   </si>
   <si>
@@ -86,9 +92,6 @@
   </si>
   <si>
     <t>Université de Picardie Jules Verne</t>
-  </si>
-  <si>
-    <t>U</t>
   </si>
   <si>
     <t>Amiens</t>
@@ -107,24 +110,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF262626"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <color rgb="FF262626"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -161,29 +165,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -471,7 +475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -480,14 +488,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="4.5703125"/>
+    <col customWidth="1" max="3" min="2" width="20.28515625"/>
+    <col customWidth="1" max="5" min="4" width="18.28515625"/>
+    <col customWidth="1" max="6" min="6" width="14.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A1" s="1">
+    <row customHeight="1" ht="51.75" r="1" spans="1:7">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -499,133 +507,133 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="51.75" r="2" spans="1:7">
+      <c r="A2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="n">
         <v>7764</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="51.75" r="3" spans="1:7">
+      <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>1709.3754</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="51.75" r="4" spans="1:7">
+      <c r="A4" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>7764</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row customHeight="1" ht="51.75" r="5" spans="1:7">
+      <c r="A5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="51.75" r="6" spans="1:7">
+      <c r="A6" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4">
-        <v>7764</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1709.3753999999999</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4">
-        <v>7764</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A5" s="1">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code refactor: - use json_db_data instead of marker data - now data is persistently added to map (markers)
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Université Bordeaux 1-IUT Agen</t>
   </si>
@@ -25,15 +25,12 @@
     <t>Agen</t>
   </si>
   <si>
+    <t>146 rue Léo Saignat, 33000 Bordeaux, France</t>
+  </si>
+  <si>
     <t>7764</t>
   </si>
   <si>
-    <t>44.802614</t>
-  </si>
-  <si>
-    <t>-0.5880540000000565</t>
-  </si>
-  <si>
     <t>Université Picardie Jules Verne-IUT Aisne</t>
   </si>
   <si>
@@ -43,10 +40,7 @@
     <t>Laon</t>
   </si>
   <si>
-    <t>49.4314025</t>
-  </si>
-  <si>
-    <t>2.0899064</t>
+    <t>54 Boulevard Saint-André, 60000 Beauvais, France</t>
   </si>
   <si>
     <t>École nationale supérieure des mines d'Albi</t>
@@ -58,10 +52,7 @@
     <t>Albi</t>
   </si>
   <si>
-    <t>43.9207561</t>
-  </si>
-  <si>
-    <t>2.1723533</t>
+    <t>Campus Jarlard, 81013 CT Cédex 09, 81000 Albi, France</t>
   </si>
   <si>
     <t>Université Paul Sabatier Toulouse 3 (UPS)-IUT Paul Sabatier-Site Albi</t>
@@ -70,40 +61,43 @@
     <t>EC</t>
   </si>
   <si>
-    <t>43.5609901</t>
-  </si>
-  <si>
-    <t>1.4630574</t>
-  </si>
-  <si>
-    <t>École nationale supérieure des mines d'Alès</t>
+    <t>31400 Toulouse, France</t>
+  </si>
+  <si>
+    <t>École des mines d'Alès</t>
   </si>
   <si>
     <t>Alès</t>
   </si>
   <si>
+    <t>30100 Alès, France</t>
+  </si>
+  <si>
     <t>3037,1709,3754,6908</t>
   </si>
   <si>
-    <t>44.13225</t>
-  </si>
-  <si>
-    <t>4.089435</t>
-  </si>
-  <si>
     <t>Université de Picardie Jules Verne</t>
   </si>
   <si>
     <t>Amiens</t>
   </si>
   <si>
+    <t>Chemin du Thil, 80000 Amiens, France</t>
+  </si>
+  <si>
     <t>convention générale</t>
   </si>
   <si>
-    <t>49.8764069</t>
-  </si>
-  <si>
-    <t>2.2637991</t>
+    <t>Université de Paris</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>75005 Paris, France</t>
+  </si>
+  <si>
+    <t>3037, 6908</t>
   </si>
 </sst>
 </file>
@@ -167,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -181,7 +175,6 @@
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -480,21 +473,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="4.5703125"/>
     <col customWidth="1" max="3" min="2" width="20.28515625"/>
-    <col customWidth="1" max="5" min="4" width="18.28515625"/>
-    <col customWidth="1" max="6" min="6" width="14.42578125"/>
+    <col customWidth="1" max="6" min="4" width="18.28515625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="51.75" r="1" spans="1:7">
+    <row customHeight="1" ht="51.75" r="1" spans="1:6">
       <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
@@ -510,126 +502,125 @@
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row customHeight="1" ht="51.75" r="2" spans="1:7">
+    <row customHeight="1" ht="51.75" r="2" spans="1:6">
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="F2" s="4" t="n">
         <v>7764</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row customHeight="1" ht="51.75" r="3" spans="1:7">
+    <row customHeight="1" ht="51.75" r="3" spans="1:6">
       <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="n">
+      <c r="F3" s="4" t="n">
         <v>1709.3754</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row customHeight="1" ht="51.75" r="4" spans="1:7">
+    <row customHeight="1" ht="51.75" r="4" spans="1:6">
       <c r="A4" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="n">
         <v>7764</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row customHeight="1" ht="51.75" r="5" spans="1:7">
+    <row customHeight="1" ht="51.75" r="5" spans="1:6">
       <c r="A5" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row customHeight="1" ht="51.75" r="6" spans="1:7">
+    <row customHeight="1" ht="52.5" r="6" spans="1:6">
       <c r="A6" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F7" t="s">
         <v>27</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code refactoring, made it cleaner, more organized and documented
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -88,7 +88,7 @@
     <t>convention générale</t>
   </si>
   <si>
-    <t>Université de Paris</t>
+    <t>Université de Paris 1</t>
   </si>
   <si>
     <t>Paris</t>
@@ -476,7 +476,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -607,6 +607,9 @@
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
another code refactor to make JS functions smaller and more readable
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Université Bordeaux 1-IUT Agen</t>
   </si>
@@ -31,6 +31,9 @@
     <t>7764</t>
   </si>
   <si>
+    <t>http://www.u-bordeaux.fr/</t>
+  </si>
+  <si>
     <t>Université Picardie Jules Verne-IUT Aisne</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t>54 Boulevard Saint-André, 60000 Beauvais, France</t>
   </si>
   <si>
+    <t>https://iut-aisne.u-picardie.fr/</t>
+  </si>
+  <si>
     <t>École nationale supérieure des mines d'Albi</t>
   </si>
   <si>
@@ -55,6 +61,9 @@
     <t>Campus Jarlard, 81013 CT Cédex 09, 81000 Albi, France</t>
   </si>
   <si>
+    <t>http://www.mines-albi.fr/</t>
+  </si>
+  <si>
     <t>Université Paul Sabatier Toulouse 3 (UPS)-IUT Paul Sabatier-Site Albi</t>
   </si>
   <si>
@@ -64,6 +73,9 @@
     <t>31400 Toulouse, France</t>
   </si>
   <si>
+    <t>http://www.univ-tlse3.fr/</t>
+  </si>
+  <si>
     <t>École nationale supérieure des mines d'Alès</t>
   </si>
   <si>
@@ -76,6 +88,9 @@
     <t>3037,1709,3754,6908</t>
   </si>
   <si>
+    <t>http://www.mines-ales.fr/</t>
+  </si>
+  <si>
     <t>Université de Picardie Jules Verne</t>
   </si>
   <si>
@@ -88,6 +103,9 @@
     <t>convention générale</t>
   </si>
   <si>
+    <t>https://www.u-picardie.fr/</t>
+  </si>
+  <si>
     <t>Université de Paris 1</t>
   </si>
   <si>
@@ -98,6 +116,9 @@
   </si>
   <si>
     <t>3037, 6908</t>
+  </si>
+  <si>
+    <t>https://www.univ-paris1.fr/</t>
   </si>
 </sst>
 </file>
@@ -105,7 +126,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -118,6 +139,12 @@
       <family val="1"/>
       <color rgb="FF262626"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="3">
@@ -158,10 +185,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -175,9 +203,11 @@
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Lien hypertexte" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -473,10 +503,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -484,9 +514,10 @@
     <col customWidth="1" max="1" min="1" width="4.5703125"/>
     <col customWidth="1" max="3" min="2" width="20.28515625"/>
     <col customWidth="1" max="6" min="4" width="18.28515625"/>
+    <col customWidth="1" max="7" min="7" width="35.140625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="51.75" r="1" spans="1:6">
+    <row customHeight="1" ht="51.75" r="1" spans="1:7">
       <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
@@ -505,125 +536,146 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="51.75" r="2" spans="1:6">
+    <row customHeight="1" ht="51.75" r="2" spans="1:7">
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>7764</v>
       </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row customHeight="1" ht="51.75" r="3" spans="1:6">
+    <row customHeight="1" ht="51.75" r="3" spans="1:7">
       <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>1709.3754</v>
       </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row customHeight="1" ht="51.75" r="4" spans="1:6">
+    <row customHeight="1" ht="51.75" r="4" spans="1:7">
       <c r="A4" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>7764</v>
       </c>
+      <c r="G4" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row customHeight="1" ht="51.75" r="5" spans="1:6">
+    <row customHeight="1" ht="51.75" r="5" spans="1:7">
       <c r="A5" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row customHeight="1" ht="52.5" r="6" spans="1:6">
+    <row customHeight="1" ht="52.5" r="6" spans="1:7">
       <c r="A6" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="n">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oops, commited bugs. now fixed.
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Université Bordeaux 1-IUT Agen</t>
   </si>
@@ -52,15 +52,15 @@
     <t>École nationale supérieure des mines d'Albi</t>
   </si>
   <si>
-    <t>EI</t>
-  </si>
-  <si>
     <t>Albi</t>
   </si>
   <si>
     <t>Campus Jarlard, 81013 CT Cédex 09, 81000 Albi, France</t>
   </si>
   <si>
+    <t>1709.3754</t>
+  </si>
+  <si>
     <t>http://www.mines-albi.fr/</t>
   </si>
   <si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>https://www.univ-paris1.fr/</t>
+  </si>
+  <si>
+    <t>Université de Lyon</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>92, rue Pasteur 30122 Lyon, France</t>
   </si>
 </sst>
 </file>
@@ -186,8 +195,8 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -206,8 +215,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Lien hypertexte" xfId="1"/>
+    <cellStyle builtinId="8" name="Lien hypertexte" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -503,7 +512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
@@ -571,16 +580,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>1709.3754</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
@@ -597,7 +606,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>18</v>
@@ -676,6 +685,26 @@
       </c>
       <c r="G7" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed edit bug where type was not correctly taken care of
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -14,44 +14,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Université Bordeaux 1-IUT Agen</t>
   </si>
   <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>Agen</t>
+  </si>
+  <si>
+    <t>146 rue Léo Saignat, 33000 Bordeaux, France</t>
+  </si>
+  <si>
+    <t>7764</t>
+  </si>
+  <si>
+    <t>http://www.u-bordeaux.fr/</t>
+  </si>
+  <si>
+    <t>Université Picardie Jules Verne-IUT Aisne</t>
+  </si>
+  <si>
+    <t>IUT</t>
+  </si>
+  <si>
+    <t>Laon</t>
+  </si>
+  <si>
+    <t>54 Boulevard Saint-André, 60000 Beauvais, France</t>
+  </si>
+  <si>
+    <t>https://iut-aisne.u-picardie.fr/</t>
+  </si>
+  <si>
+    <t>École nationale supérieure des mines d'Albi</t>
+  </si>
+  <si>
     <t>U</t>
   </si>
   <si>
-    <t>Agen</t>
-  </si>
-  <si>
-    <t>146 rue Léo Saignat, 33000 Bordeaux, France</t>
-  </si>
-  <si>
-    <t>7764</t>
-  </si>
-  <si>
-    <t>http://www.u-bordeaux.fr/</t>
-  </si>
-  <si>
-    <t>Université Picardie Jules Verne-IUT Aisne</t>
-  </si>
-  <si>
-    <t>IUT</t>
-  </si>
-  <si>
-    <t>Laon</t>
-  </si>
-  <si>
-    <t>54 Boulevard Saint-André, 60000 Beauvais, France</t>
-  </si>
-  <si>
-    <t>https://iut-aisne.u-picardie.fr/</t>
-  </si>
-  <si>
-    <t>École nationale supérieure des mines d'Albi</t>
-  </si>
-  <si>
     <t>Albi</t>
   </si>
   <si>
@@ -67,9 +70,6 @@
     <t>Université Paul Sabatier Toulouse 3 (UPS)-IUT Paul Sabatier-Site Albi</t>
   </si>
   <si>
-    <t>EC</t>
-  </si>
-  <si>
     <t>31400 Toulouse, France</t>
   </si>
   <si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>École nationale supérieure des mines d'Alès</t>
+  </si>
+  <si>
+    <t>EI</t>
   </si>
   <si>
     <t>Alès</t>
@@ -195,8 +198,8 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -215,8 +218,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Lien hypertexte" xfId="0"/>
-    <cellStyle builtinId="0" name="Normal" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Lien hypertexte" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -580,19 +583,19 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row customHeight="1" ht="51.75" r="4" spans="1:7">
@@ -600,19 +603,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="n">
-        <v>7764</v>
+      <c r="F4" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>19</v>
@@ -626,19 +629,19 @@
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row customHeight="1" ht="52.5" r="6" spans="1:7">
@@ -646,22 +649,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -669,22 +672,22 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -692,16 +695,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
fixed bug where edited data was truly edited when another Ecole was edited. Did not use the response data from the ajax call. Worked when did so.
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -52,49 +52,49 @@
     <t>École nationale supérieure des mines d'Albi</t>
   </si>
   <si>
+    <t>EI</t>
+  </si>
+  <si>
+    <t>Albi</t>
+  </si>
+  <si>
+    <t>Campus Jarlard, 81013 CT Cédex 09, 81000 Albi, France</t>
+  </si>
+  <si>
+    <t>1709.3754</t>
+  </si>
+  <si>
+    <t>http://www.mines-albi.fr/</t>
+  </si>
+  <si>
+    <t>Université Paul Sabatier Toulouse 3 (UPS)-IUT Paul Sabatier-Site Albi</t>
+  </si>
+  <si>
+    <t>31400 Toulouse, France</t>
+  </si>
+  <si>
+    <t>http://www.univ-tlse3.fr/</t>
+  </si>
+  <si>
+    <t>École nationale supérieure des mines d'Alès</t>
+  </si>
+  <si>
+    <t>Alès</t>
+  </si>
+  <si>
+    <t>30100 Alès, France</t>
+  </si>
+  <si>
+    <t>3037,1709,3754,6908</t>
+  </si>
+  <si>
+    <t>http://www.mines-ales.fr/</t>
+  </si>
+  <si>
+    <t>Université de Picardie Jules Verne</t>
+  </si>
+  <si>
     <t>U</t>
-  </si>
-  <si>
-    <t>Albi</t>
-  </si>
-  <si>
-    <t>Campus Jarlard, 81013 CT Cédex 09, 81000 Albi, France</t>
-  </si>
-  <si>
-    <t>1709.3754</t>
-  </si>
-  <si>
-    <t>http://www.mines-albi.fr/</t>
-  </si>
-  <si>
-    <t>Université Paul Sabatier Toulouse 3 (UPS)-IUT Paul Sabatier-Site Albi</t>
-  </si>
-  <si>
-    <t>31400 Toulouse, France</t>
-  </si>
-  <si>
-    <t>http://www.univ-tlse3.fr/</t>
-  </si>
-  <si>
-    <t>École nationale supérieure des mines d'Alès</t>
-  </si>
-  <si>
-    <t>EI</t>
-  </si>
-  <si>
-    <t>Alès</t>
-  </si>
-  <si>
-    <t>30100 Alès, France</t>
-  </si>
-  <si>
-    <t>3037,1709,3754,6908</t>
-  </si>
-  <si>
-    <t>http://www.mines-ales.fr/</t>
-  </si>
-  <si>
-    <t>Université de Picardie Jules Verne</t>
   </si>
   <si>
     <t>Amiens</t>
@@ -629,19 +629,19 @@
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row customHeight="1" ht="52.5" r="6" spans="1:7">
@@ -649,10 +649,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>27</v>
@@ -675,7 +675,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -698,7 +698,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
give user suggestions based on address input while typing, uses Google Maps API
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>Université Bordeaux 1-IUT Agen</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>92, rue Pasteur 30122 Lyon, France</t>
+  </si>
+  <si>
+    <t>Université d'Aix Marseille</t>
+  </si>
+  <si>
+    <t>Marseille</t>
+  </si>
+  <si>
+    <t>58, bd Charles Livon 13284 Marseille Cedex 07</t>
   </si>
 </sst>
 </file>
@@ -198,8 +207,8 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -218,8 +227,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Lien hypertexte" xfId="1"/>
+    <cellStyle builtinId="8" name="Lien hypertexte" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -515,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
@@ -710,6 +719,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>

</xml_diff>

<commit_message>
forgot to add url in edit and add forms. Now is a field
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -207,8 +207,8 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -227,8 +227,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Lien hypertexte" xfId="0"/>
-    <cellStyle builtinId="0" name="Normal" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Lien hypertexte" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>

<commit_message>
added programmes_uqac and programmes_partenaires to markers, and display both if needed in infowindow
</commit_message>
<xml_diff>
--- a/international/carte_interactive/static/carte_interactive/data/data.xlsx
+++ b/international/carte_interactive/static/carte_interactive/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="641">
   <si>
     <t>Type d'établissement</t>
   </si>
@@ -1931,6 +1931,12 @@
   </si>
   <si>
     <t>EC</t>
+  </si>
+  <si>
+    <t>1307, 7764</t>
+  </si>
+  <si>
+    <t>3037,1709,3754,6908</t>
   </si>
 </sst>
 </file>
@@ -2278,7 +2284,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2288,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L234"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E202" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K237" sqref="K237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2363,8 +2369,12 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="J2" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1">
@@ -2441,8 +2451,12 @@
         <v>16</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="1">
@@ -2551,8 +2565,12 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1">
       <c r="A10" s="1">
@@ -2603,7 +2621,9 @@
         <v>38</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1">
@@ -2687,8 +2707,12 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="A15" s="1">
@@ -2745,7 +2769,9 @@
         <v>58</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="J16" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
@@ -2885,7 +2911,9 @@
         <v>77</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1">
@@ -3021,7 +3049,9 @@
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="J26" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1">
@@ -3075,8 +3105,12 @@
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="J28" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1">
       <c r="A29" s="1">
@@ -3103,8 +3137,12 @@
         <v>105</v>
       </c>
       <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="J29" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1">
       <c r="A30" s="1">
@@ -3211,7 +3249,9 @@
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="J33" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1">
@@ -3315,7 +3355,9 @@
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
+      <c r="J37" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" ht="15" customHeight="1">
@@ -3395,8 +3437,12 @@
         <v>138</v>
       </c>
       <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="J40" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1">
       <c r="A41" s="1">
@@ -3489,8 +3535,12 @@
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
+      <c r="J44" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1">
       <c r="A45" s="1">
@@ -3593,7 +3643,9 @@
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="J48" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11" ht="15" customHeight="1">
@@ -3751,7 +3803,9 @@
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
+      <c r="J54" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K54" s="2"/>
     </row>
     <row r="55" spans="1:11" ht="15" customHeight="1">
@@ -3897,8 +3951,12 @@
         <v>199</v>
       </c>
       <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
+      <c r="J59" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K59" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="60" spans="1:11" ht="15" customHeight="1">
       <c r="A60" s="1">
@@ -3983,8 +4041,12 @@
         <v>211</v>
       </c>
       <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
+      <c r="J62" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K62" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="63" spans="1:11" ht="15" customHeight="1">
       <c r="A63" s="1">
@@ -4011,7 +4073,9 @@
         <v>215</v>
       </c>
       <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
+      <c r="J63" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:11" ht="15" customHeight="1">
@@ -4179,7 +4243,9 @@
         <v>238</v>
       </c>
       <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
+      <c r="J69" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K69" s="2"/>
     </row>
     <row r="70" spans="1:11" ht="15" customHeight="1">
@@ -4309,8 +4375,12 @@
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
+      <c r="J74" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K74" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="75" spans="1:11" ht="15" customHeight="1">
       <c r="A75" s="1">
@@ -4443,8 +4513,12 @@
         <v>268</v>
       </c>
       <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
+      <c r="J79" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K79" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="80" spans="1:11" ht="15" customHeight="1">
       <c r="A80" s="1">
@@ -4495,7 +4569,9 @@
         <v>273</v>
       </c>
       <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
+      <c r="J81" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K81" s="2"/>
     </row>
     <row r="82" spans="1:11" ht="15" customHeight="1">
@@ -4599,7 +4675,9 @@
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
+      <c r="J85" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K85" s="2"/>
     </row>
     <row r="86" spans="1:11" ht="15" customHeight="1">
@@ -4695,7 +4773,9 @@
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
+      <c r="J89" s="2" t="s">
+        <v>639</v>
+      </c>
       <c r="K89" s="2"/>
     </row>
     <row r="90" spans="1:11" ht="15" customHeight="1">
@@ -4819,7 +4899,9 @@
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
+      <c r="J94" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K94" s="2"/>
     </row>
     <row r="95" spans="1:11" ht="15" customHeight="1">
@@ -4897,8 +4979,12 @@
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
+      <c r="J97" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K97" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="98" spans="1:11" ht="15" customHeight="1">
       <c r="A98" s="1">
@@ -4973,7 +5059,9 @@
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
+      <c r="J100" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K100" s="2"/>
     </row>
     <row r="101" spans="1:11" ht="15" customHeight="1">
@@ -5019,7 +5107,9 @@
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
+      <c r="J102" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K102" s="2"/>
     </row>
     <row r="103" spans="1:11" ht="15" customHeight="1">
@@ -5145,8 +5235,12 @@
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
+      <c r="J107" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K107" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="108" spans="1:11" ht="15" customHeight="1">
       <c r="A108" s="1">
@@ -5253,7 +5347,9 @@
         <v>348</v>
       </c>
       <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
+      <c r="J111" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K111" s="2"/>
     </row>
     <row r="112" spans="1:11" ht="15" customHeight="1">
@@ -5357,8 +5453,12 @@
         <v>359</v>
       </c>
       <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
+      <c r="J115" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K115" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="116" spans="1:11" ht="15" customHeight="1">
       <c r="A116" s="1">
@@ -5411,7 +5511,9 @@
         <v>105</v>
       </c>
       <c r="I117" s="2"/>
-      <c r="J117" s="2"/>
+      <c r="J117" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K117" s="2"/>
     </row>
     <row r="118" spans="1:11" ht="15" customHeight="1">
@@ -5463,8 +5565,12 @@
         <v>370</v>
       </c>
       <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
+      <c r="J119" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K119" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="120" spans="1:11" ht="15" customHeight="1">
       <c r="A120" s="1">
@@ -5653,7 +5759,9 @@
       </c>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
-      <c r="J126" s="2"/>
+      <c r="J126" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K126" s="2"/>
     </row>
     <row r="127" spans="1:11" ht="15" customHeight="1">
@@ -5849,8 +5957,12 @@
         <v>418</v>
       </c>
       <c r="I133" s="2"/>
-      <c r="J133" s="2"/>
-      <c r="K133" s="2"/>
+      <c r="J133" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K133" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="134" spans="1:11" ht="15" customHeight="1">
       <c r="A134" s="1">
@@ -5955,8 +6067,12 @@
         <v>431</v>
       </c>
       <c r="I137" s="2"/>
-      <c r="J137" s="2"/>
-      <c r="K137" s="2"/>
+      <c r="J137" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K137" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="138" spans="1:11" ht="15" customHeight="1">
       <c r="A138" s="1">
@@ -6031,7 +6147,9 @@
       </c>
       <c r="H140" s="2"/>
       <c r="I140" s="2"/>
-      <c r="J140" s="2"/>
+      <c r="J140" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K140" s="2"/>
     </row>
     <row r="141" spans="1:11" ht="15" customHeight="1">
@@ -6085,7 +6203,9 @@
       </c>
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
-      <c r="J142" s="2"/>
+      <c r="J142" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K142" s="2"/>
     </row>
     <row r="143" spans="1:11" ht="15" customHeight="1">
@@ -6165,8 +6285,12 @@
         <v>452</v>
       </c>
       <c r="I145" s="2"/>
-      <c r="J145" s="2"/>
-      <c r="K145" s="2"/>
+      <c r="J145" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K145" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="146" spans="1:11" ht="15" customHeight="1">
       <c r="A146" s="1">
@@ -6361,7 +6485,9 @@
         <v>403</v>
       </c>
       <c r="I153" s="2"/>
-      <c r="J153" s="2"/>
+      <c r="J153" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K153" s="2"/>
     </row>
     <row r="154" spans="1:11" ht="15" customHeight="1">
@@ -6415,8 +6541,12 @@
       </c>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
-      <c r="J155" s="2"/>
-      <c r="K155" s="2"/>
+      <c r="J155" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K155" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="156" spans="1:11" ht="15" customHeight="1">
       <c r="A156" s="1">
@@ -6487,7 +6617,9 @@
       </c>
       <c r="H158" s="2"/>
       <c r="I158" s="2"/>
-      <c r="J158" s="2"/>
+      <c r="J158" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K158" s="2"/>
     </row>
     <row r="159" spans="1:11" ht="15" customHeight="1">
@@ -6543,8 +6675,12 @@
         <v>486</v>
       </c>
       <c r="I160" s="2"/>
-      <c r="J160" s="2"/>
-      <c r="K160" s="2"/>
+      <c r="J160" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K160" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="161" spans="1:11" ht="15" customHeight="1">
       <c r="A161" s="1">
@@ -6623,7 +6759,9 @@
         <v>494</v>
       </c>
       <c r="I163" s="2"/>
-      <c r="J163" s="2"/>
+      <c r="J163" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K163" s="2"/>
     </row>
     <row r="164" spans="1:11" ht="15" customHeight="1">
@@ -6679,7 +6817,9 @@
         <v>501</v>
       </c>
       <c r="I165" s="2"/>
-      <c r="J165" s="2"/>
+      <c r="J165" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K165" s="2"/>
     </row>
     <row r="166" spans="1:11" ht="15" customHeight="1">
@@ -6819,8 +6959,12 @@
         <v>517</v>
       </c>
       <c r="I170" s="2"/>
-      <c r="J170" s="2"/>
-      <c r="K170" s="2"/>
+      <c r="J170" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K170" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="171" spans="1:11" ht="15" customHeight="1">
       <c r="A171" s="1">
@@ -6969,7 +7113,9 @@
       </c>
       <c r="H176" s="2"/>
       <c r="I176" s="2"/>
-      <c r="J176" s="2"/>
+      <c r="J176" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K176" s="2"/>
     </row>
     <row r="177" spans="1:11" ht="15" customHeight="1">
@@ -7021,8 +7167,12 @@
       </c>
       <c r="H178" s="2"/>
       <c r="I178" s="2"/>
-      <c r="J178" s="2"/>
-      <c r="K178" s="2"/>
+      <c r="J178" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K178" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="179" spans="1:11" ht="15" customHeight="1">
       <c r="A179" s="1">
@@ -7143,7 +7293,9 @@
       </c>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
-      <c r="J183" s="2"/>
+      <c r="J183" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K183" s="2"/>
     </row>
     <row r="184" spans="1:11" ht="15" customHeight="1">
@@ -7191,8 +7343,12 @@
       </c>
       <c r="H185" s="2"/>
       <c r="I185" s="2"/>
-      <c r="J185" s="2"/>
-      <c r="K185" s="2"/>
+      <c r="J185" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K185" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="186" spans="1:11" ht="15" customHeight="1">
       <c r="A186" s="1">
@@ -7239,7 +7395,9 @@
       </c>
       <c r="H187" s="2"/>
       <c r="I187" s="2"/>
-      <c r="J187" s="2"/>
+      <c r="J187" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K187" s="2"/>
     </row>
     <row r="188" spans="1:11" ht="15" customHeight="1">
@@ -7457,8 +7615,12 @@
       </c>
       <c r="H196" s="2"/>
       <c r="I196" s="2"/>
-      <c r="J196" s="2"/>
-      <c r="K196" s="2"/>
+      <c r="J196" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K196" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="197" spans="1:11" ht="15" customHeight="1">
       <c r="A197" s="1">
@@ -7505,7 +7667,9 @@
       </c>
       <c r="H198" s="2"/>
       <c r="I198" s="2"/>
-      <c r="J198" s="2"/>
+      <c r="J198" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K198" s="2"/>
     </row>
     <row r="199" spans="1:11" ht="15" customHeight="1">
@@ -7637,8 +7801,12 @@
       </c>
       <c r="H203" s="2"/>
       <c r="I203" s="2"/>
-      <c r="J203" s="2"/>
-      <c r="K203" s="2"/>
+      <c r="J203" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K203" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="204" spans="1:11" ht="15" customHeight="1">
       <c r="A204" s="1">
@@ -7739,7 +7907,9 @@
       </c>
       <c r="H207" s="2"/>
       <c r="I207" s="2"/>
-      <c r="J207" s="2"/>
+      <c r="J207" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K207" s="2"/>
     </row>
     <row r="208" spans="1:11" ht="15" customHeight="1">
@@ -7885,7 +8055,9 @@
       </c>
       <c r="H213" s="2"/>
       <c r="I213" s="2"/>
-      <c r="J213" s="2"/>
+      <c r="J213" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K213" s="2"/>
     </row>
     <row r="214" spans="1:11" ht="15" customHeight="1">
@@ -7991,8 +8163,12 @@
       </c>
       <c r="H217" s="2"/>
       <c r="I217" s="2"/>
-      <c r="J217" s="2"/>
-      <c r="K217" s="2"/>
+      <c r="J217" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K217" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="218" spans="1:11" ht="15" customHeight="1">
       <c r="A218" s="1">
@@ -8089,8 +8265,12 @@
       </c>
       <c r="H221" s="2"/>
       <c r="I221" s="2"/>
-      <c r="J221" s="2"/>
-      <c r="K221" s="2"/>
+      <c r="J221" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K221" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="222" spans="1:11" ht="15" customHeight="1">
       <c r="A222" s="1">
@@ -8245,7 +8425,9 @@
         <v>615</v>
       </c>
       <c r="I227" s="2"/>
-      <c r="J227" s="2"/>
+      <c r="J227" s="2" t="s">
+        <v>640</v>
+      </c>
       <c r="K227" s="2"/>
     </row>
     <row r="228" spans="1:11" ht="15" customHeight="1">
@@ -8295,7 +8477,9 @@
       </c>
       <c r="H229" s="2"/>
       <c r="I229" s="2"/>
-      <c r="J229" s="2"/>
+      <c r="J229" s="2">
+        <v>1709.3753999999999</v>
+      </c>
       <c r="K229" s="2"/>
     </row>
     <row r="230" spans="1:11" ht="15" customHeight="1">
@@ -8401,8 +8585,12 @@
         <v>31000</v>
       </c>
       <c r="I233" s="2"/>
-      <c r="J233" s="2"/>
-      <c r="K233" s="2"/>
+      <c r="J233" s="2">
+        <v>7764</v>
+      </c>
+      <c r="K233" s="2">
+        <v>1234</v>
+      </c>
     </row>
     <row r="234" spans="1:11" ht="15" customHeight="1">
       <c r="A234" s="1">
@@ -8429,8 +8617,12 @@
         <v>31042</v>
       </c>
       <c r="I234" s="2"/>
-      <c r="J234" s="2"/>
-      <c r="K234" s="2"/>
+      <c r="J234" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K234" s="2">
+        <v>1234</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>